<commit_message>
;merge=X  for Excel files
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_02_excel_a_xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_02_excel_a_xlsx.w3mi.data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MoldaB\Desktop\save\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,10 +15,7 @@
     <sheet name="NoGroup" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="E_">#REF!</definedName>
-    <definedName name="F_">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">NoGroup!$3:$4</definedName>
-    <definedName name="RANGE_SUM1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -543,6 +540,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>